<commit_message>
Génération du maillage octogonal OK (2x2 pixels). Mise à jour du fichier excel correspondant pour le rapport.
</commit_message>
<xml_diff>
--- a/documents/maillage_perfs.xlsx
+++ b/documents/maillage_perfs.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>temps [s]</t>
   </si>
@@ -38,13 +38,27 @@
   <si>
     <t>nœuds + arcs</t>
   </si>
+  <si>
+    <t>nb nœuds</t>
+  </si>
+  <si>
+    <t>Pour des nœuds représentant 2x2 pixels</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+  <fonts count="2">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -60,7 +74,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -68,13 +82,59 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -102,7 +162,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Feuil1!$D$2</c:f>
+              <c:f>Feuil1!$D$5</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -114,14 +174,6 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
-          <c:trendline>
-            <c:trendlineType val="power"/>
-            <c:dispEq val="1"/>
-            <c:trendlineLbl>
-              <c:layout/>
-              <c:numFmt formatCode="General" sourceLinked="0"/>
-            </c:trendlineLbl>
-          </c:trendline>
           <c:trendline>
             <c:trendlineType val="poly"/>
             <c:order val="2"/>
@@ -133,7 +185,7 @@
           </c:trendline>
           <c:cat>
             <c:multiLvlStrRef>
-              <c:f>Feuil1!$A$3:$B$17</c:f>
+              <c:f>Feuil1!$A$6:$B$20</c:f>
               <c:multiLvlStrCache>
                 <c:ptCount val="15"/>
                 <c:lvl>
@@ -188,43 +240,43 @@
                     <c:v>0</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>75</c:v>
+                    <c:v>80</c:v>
                   </c:pt>
                   <c:pt idx="2">
                     <c:v>150</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>225</c:v>
+                    <c:v>220</c:v>
                   </c:pt>
                   <c:pt idx="4">
                     <c:v>300</c:v>
                   </c:pt>
                   <c:pt idx="5">
-                    <c:v>375</c:v>
+                    <c:v>380</c:v>
                   </c:pt>
                   <c:pt idx="6">
                     <c:v>450</c:v>
                   </c:pt>
                   <c:pt idx="7">
-                    <c:v>525</c:v>
+                    <c:v>530</c:v>
                   </c:pt>
                   <c:pt idx="8">
                     <c:v>600</c:v>
                   </c:pt>
                   <c:pt idx="9">
-                    <c:v>675</c:v>
+                    <c:v>680</c:v>
                   </c:pt>
                   <c:pt idx="10">
-                    <c:v>750</c:v>
+                    <c:v>760</c:v>
                   </c:pt>
                   <c:pt idx="11">
-                    <c:v>825</c:v>
+                    <c:v>830</c:v>
                   </c:pt>
                   <c:pt idx="12">
                     <c:v>900</c:v>
                   </c:pt>
                   <c:pt idx="13">
-                    <c:v>975</c:v>
+                    <c:v>980</c:v>
                   </c:pt>
                   <c:pt idx="14">
                     <c:v>1050</c:v>
@@ -235,7 +287,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Feuil1!$D$3:$D$17</c:f>
+              <c:f>Feuil1!$D$6:$D$20</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
@@ -243,71 +295,70 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>7.8E-2</c:v>
+                  <c:v>6.2E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>0.109</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>0.25</c:v>
                 </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.57799999999999996</c:v>
-                </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.109</c:v>
+                  <c:v>0.45300000000000001</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.734</c:v>
+                  <c:v>0.68799999999999994</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2.5470000000000002</c:v>
+                  <c:v>1.0780000000000001</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>4.7190000000000003</c:v>
+                  <c:v>1.5</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>6.141</c:v>
+                  <c:v>2.109</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>7.532</c:v>
+                  <c:v>2.6869999999999998</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>11.484</c:v>
+                  <c:v>3.36</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>13.452999999999999</c:v>
+                  <c:v>5.2649999999999997</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>18.375</c:v>
+                  <c:v>6.0309999999999997</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>20.327999999999999</c:v>
+                  <c:v>7.0780000000000003</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>22.859000000000002</c:v>
+                  <c:v>8.0619999999999994</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="112786816"/>
-        <c:axId val="113486080"/>
+        <c:axId val="90383872"/>
+        <c:axId val="90385408"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="112786816"/>
+        <c:axId val="90383872"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="113486080"/>
+        <c:crossAx val="90385408"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="113486080"/>
+        <c:axId val="90385408"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -315,24 +366,20 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="112786816"/>
+        <c:crossAx val="90383872"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:legendEntry>
-        <c:idx val="1"/>
-        <c:delete val="1"/>
-      </c:legendEntry>
       <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -354,7 +401,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Feuil1!$E$2</c:f>
+              <c:f>Feuil1!$E$5</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -377,7 +424,7 @@
           </c:trendline>
           <c:cat>
             <c:multiLvlStrRef>
-              <c:f>Feuil1!$A$3:$B$17</c:f>
+              <c:f>Feuil1!$A$6:$B$20</c:f>
               <c:multiLvlStrCache>
                 <c:ptCount val="15"/>
                 <c:lvl>
@@ -432,43 +479,43 @@
                     <c:v>0</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>75</c:v>
+                    <c:v>80</c:v>
                   </c:pt>
                   <c:pt idx="2">
                     <c:v>150</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>225</c:v>
+                    <c:v>220</c:v>
                   </c:pt>
                   <c:pt idx="4">
                     <c:v>300</c:v>
                   </c:pt>
                   <c:pt idx="5">
-                    <c:v>375</c:v>
+                    <c:v>380</c:v>
                   </c:pt>
                   <c:pt idx="6">
                     <c:v>450</c:v>
                   </c:pt>
                   <c:pt idx="7">
-                    <c:v>525</c:v>
+                    <c:v>530</c:v>
                   </c:pt>
                   <c:pt idx="8">
                     <c:v>600</c:v>
                   </c:pt>
                   <c:pt idx="9">
-                    <c:v>675</c:v>
+                    <c:v>680</c:v>
                   </c:pt>
                   <c:pt idx="10">
-                    <c:v>750</c:v>
+                    <c:v>760</c:v>
                   </c:pt>
                   <c:pt idx="11">
-                    <c:v>825</c:v>
+                    <c:v>830</c:v>
                   </c:pt>
                   <c:pt idx="12">
                     <c:v>900</c:v>
                   </c:pt>
                   <c:pt idx="13">
-                    <c:v>975</c:v>
+                    <c:v>980</c:v>
                   </c:pt>
                   <c:pt idx="14">
                     <c:v>1050</c:v>
@@ -479,7 +526,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Feuil1!$E$3:$E$17</c:f>
+              <c:f>Feuil1!$E$6:$E$20</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
@@ -487,71 +534,70 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3.63</c:v>
+                  <c:v>1.94</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>11.13</c:v>
+                  <c:v>5.47</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>23.28</c:v>
+                  <c:v>8.67</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>41.45</c:v>
+                  <c:v>15.72</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>62.14</c:v>
+                  <c:v>24.53</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>94.81</c:v>
+                  <c:v>35.22</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>114.85</c:v>
+                  <c:v>48.25</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>166.4</c:v>
+                  <c:v>65.37</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>206.1</c:v>
+                  <c:v>81.790000000000006</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>242.55</c:v>
+                  <c:v>98.91</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>313.92</c:v>
+                  <c:v>107.21</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>350.44</c:v>
+                  <c:v>130.72999999999999</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>425.84</c:v>
+                  <c:v>158.19</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>489.75</c:v>
+                  <c:v>184.83</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="115038848"/>
-        <c:axId val="115156096"/>
+        <c:axId val="51421952"/>
+        <c:axId val="51423488"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="115038848"/>
+        <c:axId val="51421952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="115156096"/>
+        <c:crossAx val="51423488"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="115156096"/>
+        <c:axId val="51423488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -559,7 +605,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="115038848"/>
+        <c:crossAx val="51421952"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -583,19 +629,19 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>238124</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>85725</xdr:rowOff>
+      <xdr:colOff>114299</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>133349</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>923924</xdr:colOff>
-      <xdr:row>39</xdr:row>
-      <xdr:rowOff>114299</xdr:rowOff>
+      <xdr:colOff>981075</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="7" name="Graphique 6"/>
+        <xdr:cNvPr id="5" name="Graphique 4"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -612,20 +658,20 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>9524</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>95249</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>1095374</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>114299</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>295275</xdr:colOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>733425</xdr:colOff>
       <xdr:row>39</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:rowOff>28575</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="8" name="Graphique 7"/>
+        <xdr:cNvPr id="6" name="Graphique 5"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -928,10 +974,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A2:G17"/>
+  <dimension ref="A2:I20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:A17"/>
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -942,436 +988,493 @@
     <col min="5" max="5" width="15.5703125" style="1" customWidth="1"/>
     <col min="6" max="6" width="11.42578125" style="1"/>
     <col min="7" max="7" width="16.5703125" style="1" customWidth="1"/>
-    <col min="8" max="16384" width="11.42578125" style="1"/>
+    <col min="8" max="8" width="14" style="1" customWidth="1"/>
+    <col min="9" max="16384" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:7">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:9">
+      <c r="B2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
+      <c r="I2" s="4"/>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="A5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" s="1" t="s">
+      <c r="C5" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D5" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E5" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="F5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="G5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H5" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
-      <c r="A3" s="1">
-        <f>B3*3/4</f>
+    <row r="6" spans="1:9">
+      <c r="A6" s="1">
+        <f>B6*3/4</f>
         <v>0</v>
       </c>
-      <c r="B3" s="1">
+      <c r="B6" s="1">
         <v>0</v>
       </c>
-      <c r="C3" s="1">
+      <c r="C6" s="1">
         <v>0</v>
       </c>
-      <c r="D3" s="1">
+      <c r="D6" s="1">
         <v>0</v>
       </c>
-      <c r="E3" s="1">
+      <c r="E6" s="1">
         <v>0</v>
       </c>
-      <c r="F3" s="1">
+      <c r="F6" s="1">
         <v>0</v>
       </c>
-      <c r="G3" s="1">
-        <f>C3+F3</f>
+      <c r="G6" s="1">
+        <f t="shared" ref="G6:G9" si="0">C6/4</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:7">
-      <c r="A4" s="1">
-        <f t="shared" ref="A4:A17" si="0">B4*3/4</f>
-        <v>75</v>
-      </c>
-      <c r="B4" s="1">
+      <c r="H6" s="1">
+        <f>F6+G6</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
+      <c r="A7" s="1">
+        <v>80</v>
+      </c>
+      <c r="B7" s="1">
         <v>100</v>
       </c>
-      <c r="C4" s="1">
-        <f>A4*B4</f>
+      <c r="C7" s="1">
+        <f t="shared" ref="C7:C20" si="1">A7*B7</f>
+        <v>8000</v>
+      </c>
+      <c r="D7" s="1">
+        <v>6.2E-2</v>
+      </c>
+      <c r="E7" s="1">
+        <v>1.94</v>
+      </c>
+      <c r="F7" s="1">
+        <v>7141</v>
+      </c>
+      <c r="G7" s="1">
+        <f t="shared" si="0"/>
+        <v>2000</v>
+      </c>
+      <c r="H7" s="1">
+        <f t="shared" ref="H7:H20" si="2">F7+G7</f>
+        <v>9141</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
+      <c r="A8" s="1">
+        <f t="shared" ref="A7:A20" si="3">B8*3/4</f>
+        <v>150</v>
+      </c>
+      <c r="B8" s="1">
+        <v>200</v>
+      </c>
+      <c r="C8" s="1">
+        <f t="shared" si="1"/>
+        <v>30000</v>
+      </c>
+      <c r="D8" s="1">
+        <v>0.109</v>
+      </c>
+      <c r="E8" s="1">
+        <v>5.47</v>
+      </c>
+      <c r="F8" s="1">
+        <v>29477</v>
+      </c>
+      <c r="G8" s="1">
+        <f t="shared" si="0"/>
         <v>7500</v>
       </c>
-      <c r="D4" s="1">
-        <v>7.8E-2</v>
-      </c>
-      <c r="E4" s="1">
-        <v>3.63</v>
-      </c>
-      <c r="F4" s="1">
-        <f>2*C4-(A4+B4)</f>
-        <v>14825</v>
-      </c>
-      <c r="G4" s="1">
-        <f t="shared" ref="G4:G17" si="1">C4+F4</f>
-        <v>22325</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7">
-      <c r="A5" s="1">
+      <c r="H8" s="1">
+        <f t="shared" si="2"/>
+        <v>36977</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
+      <c r="A9" s="1">
+        <v>220</v>
+      </c>
+      <c r="B9" s="1">
+        <v>300</v>
+      </c>
+      <c r="C9" s="1">
+        <f t="shared" si="1"/>
+        <v>66000</v>
+      </c>
+      <c r="D9" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="E9" s="1">
+        <v>8.67</v>
+      </c>
+      <c r="F9" s="1">
+        <v>65222</v>
+      </c>
+      <c r="G9" s="1">
         <f t="shared" si="0"/>
-        <v>150</v>
-      </c>
-      <c r="B5" s="1">
-        <v>200</v>
-      </c>
-      <c r="C5" s="1">
-        <f>A5*B5</f>
+        <v>16500</v>
+      </c>
+      <c r="H9" s="1">
+        <f t="shared" si="2"/>
+        <v>81722</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
+      <c r="A10" s="1">
+        <f t="shared" si="3"/>
+        <v>300</v>
+      </c>
+      <c r="B10" s="1">
+        <v>400</v>
+      </c>
+      <c r="C10" s="1">
+        <f t="shared" si="1"/>
+        <v>120000</v>
+      </c>
+      <c r="D10" s="1">
+        <v>0.45300000000000001</v>
+      </c>
+      <c r="E10" s="1">
+        <v>15.72</v>
+      </c>
+      <c r="F10" s="1">
+        <v>118952</v>
+      </c>
+      <c r="G10" s="1">
+        <f>C10/4</f>
         <v>30000</v>
       </c>
-      <c r="D5" s="1">
-        <v>0.25</v>
-      </c>
-      <c r="E5" s="1">
-        <v>11.13</v>
-      </c>
-      <c r="F5" s="1">
-        <f>2*C5-(A5+B5)</f>
-        <v>59650</v>
-      </c>
-      <c r="G5" s="1">
+      <c r="H10" s="1">
+        <f t="shared" si="2"/>
+        <v>148952</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9">
+      <c r="A11" s="1">
+        <v>380</v>
+      </c>
+      <c r="B11" s="1">
+        <v>500</v>
+      </c>
+      <c r="C11" s="1">
         <f t="shared" si="1"/>
-        <v>89650</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7">
-      <c r="A6" s="1">
-        <f t="shared" si="0"/>
-        <v>225</v>
-      </c>
-      <c r="B6" s="1">
-        <v>300</v>
-      </c>
-      <c r="C6" s="1">
-        <f>A6*B6</f>
+        <v>190000</v>
+      </c>
+      <c r="D11" s="1">
+        <v>0.68799999999999994</v>
+      </c>
+      <c r="E11" s="1">
+        <v>24.53</v>
+      </c>
+      <c r="F11" s="1">
+        <v>188682</v>
+      </c>
+      <c r="G11" s="1">
+        <f t="shared" ref="G11:G20" si="4">C11/4</f>
+        <v>47500</v>
+      </c>
+      <c r="H11" s="1">
+        <f t="shared" si="2"/>
+        <v>236182</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9">
+      <c r="A12" s="1">
+        <f t="shared" si="3"/>
+        <v>450</v>
+      </c>
+      <c r="B12" s="1">
+        <v>600</v>
+      </c>
+      <c r="C12" s="1">
+        <f t="shared" si="1"/>
+        <v>270000</v>
+      </c>
+      <c r="D12" s="1">
+        <v>1.0780000000000001</v>
+      </c>
+      <c r="E12" s="1">
+        <v>35.22</v>
+      </c>
+      <c r="F12" s="1">
+        <v>268427</v>
+      </c>
+      <c r="G12" s="1">
+        <f t="shared" si="4"/>
         <v>67500</v>
       </c>
-      <c r="D6" s="1">
-        <v>0.57799999999999996</v>
-      </c>
-      <c r="E6" s="1">
-        <v>23.28</v>
-      </c>
-      <c r="F6" s="1">
-        <f>2*C6-(A6+B6)</f>
-        <v>134475</v>
-      </c>
-      <c r="G6" s="1">
+      <c r="H12" s="1">
+        <f t="shared" si="2"/>
+        <v>335927</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9">
+      <c r="A13" s="1">
+        <v>530</v>
+      </c>
+      <c r="B13" s="1">
+        <v>700</v>
+      </c>
+      <c r="C13" s="1">
         <f t="shared" si="1"/>
-        <v>201975</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7">
-      <c r="A7" s="1">
-        <f t="shared" si="0"/>
-        <v>300</v>
-      </c>
-      <c r="B7" s="1">
-        <v>400</v>
-      </c>
-      <c r="C7" s="1">
-        <f>A7*B7</f>
+        <v>371000</v>
+      </c>
+      <c r="D13" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="E13" s="1">
+        <v>48.25</v>
+      </c>
+      <c r="F13" s="1">
+        <v>369157</v>
+      </c>
+      <c r="G13" s="1">
+        <f t="shared" si="4"/>
+        <v>92750</v>
+      </c>
+      <c r="H13" s="1">
+        <f t="shared" si="2"/>
+        <v>461907</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9">
+      <c r="A14" s="1">
+        <f t="shared" si="3"/>
+        <v>600</v>
+      </c>
+      <c r="B14" s="1">
+        <v>800</v>
+      </c>
+      <c r="C14" s="1">
+        <f t="shared" si="1"/>
+        <v>480000</v>
+      </c>
+      <c r="D14" s="1">
+        <v>2.109</v>
+      </c>
+      <c r="E14" s="1">
+        <v>65.37</v>
+      </c>
+      <c r="F14" s="1">
+        <v>477902</v>
+      </c>
+      <c r="G14" s="1">
+        <f t="shared" si="4"/>
         <v>120000</v>
       </c>
-      <c r="D7" s="1">
-        <v>1.109</v>
-      </c>
-      <c r="E7" s="1">
-        <v>41.45</v>
-      </c>
-      <c r="F7" s="1">
-        <f>2*C7-(A7+B7)</f>
-        <v>239300</v>
-      </c>
-      <c r="G7" s="1">
+      <c r="H14" s="1">
+        <f t="shared" si="2"/>
+        <v>597902</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9">
+      <c r="A15" s="1">
+        <v>680</v>
+      </c>
+      <c r="B15" s="1">
+        <v>900</v>
+      </c>
+      <c r="C15" s="1">
         <f t="shared" si="1"/>
-        <v>359300</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7">
-      <c r="A8" s="1">
-        <f t="shared" si="0"/>
-        <v>375</v>
-      </c>
-      <c r="B8" s="1">
-        <v>500</v>
-      </c>
-      <c r="C8" s="1">
-        <f>A8*B8</f>
-        <v>187500</v>
-      </c>
-      <c r="D8" s="1">
-        <v>1.734</v>
-      </c>
-      <c r="E8" s="1">
-        <v>62.14</v>
-      </c>
-      <c r="F8" s="1">
-        <f>2*C8-(A8+B8)</f>
-        <v>374125</v>
-      </c>
-      <c r="G8" s="1">
+        <v>612000</v>
+      </c>
+      <c r="D15" s="1">
+        <v>2.6869999999999998</v>
+      </c>
+      <c r="E15" s="1">
+        <v>81.790000000000006</v>
+      </c>
+      <c r="F15" s="1">
+        <v>609632</v>
+      </c>
+      <c r="G15" s="1">
+        <f t="shared" si="4"/>
+        <v>153000</v>
+      </c>
+      <c r="H15" s="1">
+        <f t="shared" si="2"/>
+        <v>762632</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9">
+      <c r="A16" s="1">
+        <v>760</v>
+      </c>
+      <c r="B16" s="1">
+        <v>1000</v>
+      </c>
+      <c r="C16" s="1">
         <f t="shared" si="1"/>
-        <v>561625</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7">
-      <c r="A9" s="1">
-        <f t="shared" si="0"/>
-        <v>450</v>
-      </c>
-      <c r="B9" s="1">
-        <v>600</v>
-      </c>
-      <c r="C9" s="1">
-        <f>A9*B9</f>
+        <v>760000</v>
+      </c>
+      <c r="D16" s="1">
+        <v>3.36</v>
+      </c>
+      <c r="E16" s="1">
+        <v>98.91</v>
+      </c>
+      <c r="F16" s="1">
+        <v>757362</v>
+      </c>
+      <c r="G16" s="1">
+        <f t="shared" si="4"/>
+        <v>190000</v>
+      </c>
+      <c r="H16" s="1">
+        <f t="shared" si="2"/>
+        <v>947362</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8">
+      <c r="A17" s="1">
+        <v>830</v>
+      </c>
+      <c r="B17" s="1">
+        <v>1100</v>
+      </c>
+      <c r="C17" s="1">
+        <f t="shared" si="1"/>
+        <v>913000</v>
+      </c>
+      <c r="D17" s="1">
+        <v>5.2649999999999997</v>
+      </c>
+      <c r="E17" s="1">
+        <v>107.21</v>
+      </c>
+      <c r="F17" s="1">
+        <v>910107</v>
+      </c>
+      <c r="G17" s="1">
+        <f t="shared" si="4"/>
+        <v>228250</v>
+      </c>
+      <c r="H17" s="1">
+        <f t="shared" si="2"/>
+        <v>1138357</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8">
+      <c r="A18" s="1">
+        <f t="shared" si="3"/>
+        <v>900</v>
+      </c>
+      <c r="B18" s="1">
+        <v>1200</v>
+      </c>
+      <c r="C18" s="1">
+        <f t="shared" si="1"/>
+        <v>1080000</v>
+      </c>
+      <c r="D18" s="1">
+        <v>6.0309999999999997</v>
+      </c>
+      <c r="E18" s="1">
+        <v>130.72999999999999</v>
+      </c>
+      <c r="F18" s="1">
+        <v>1076852</v>
+      </c>
+      <c r="G18" s="1">
+        <f t="shared" si="4"/>
         <v>270000</v>
       </c>
-      <c r="D9" s="1">
-        <v>2.5470000000000002</v>
-      </c>
-      <c r="E9" s="1">
-        <v>94.81</v>
-      </c>
-      <c r="F9" s="1">
-        <f>2*C9-(A9+B9)</f>
-        <v>538950</v>
-      </c>
-      <c r="G9" s="1">
+      <c r="H18" s="1">
+        <f t="shared" si="2"/>
+        <v>1346852</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8">
+      <c r="A19" s="1">
+        <v>980</v>
+      </c>
+      <c r="B19" s="1">
+        <v>1300</v>
+      </c>
+      <c r="C19" s="1">
         <f t="shared" si="1"/>
-        <v>808950</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7">
-      <c r="A10" s="1">
-        <f t="shared" si="0"/>
-        <v>525</v>
-      </c>
-      <c r="B10" s="1">
-        <v>700</v>
-      </c>
-      <c r="C10" s="1">
-        <f>A10*B10</f>
+        <v>1274000</v>
+      </c>
+      <c r="D19" s="1">
+        <v>7.0780000000000003</v>
+      </c>
+      <c r="E19" s="1">
+        <v>158.19</v>
+      </c>
+      <c r="F19" s="1">
+        <v>1270582</v>
+      </c>
+      <c r="G19" s="1">
+        <f t="shared" si="4"/>
+        <v>318500</v>
+      </c>
+      <c r="H19" s="1">
+        <f t="shared" si="2"/>
+        <v>1589082</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8">
+      <c r="A20" s="1">
+        <f t="shared" si="3"/>
+        <v>1050</v>
+      </c>
+      <c r="B20" s="1">
+        <v>1400</v>
+      </c>
+      <c r="C20" s="1">
+        <f t="shared" si="1"/>
+        <v>1470000</v>
+      </c>
+      <c r="D20" s="1">
+        <v>8.0619999999999994</v>
+      </c>
+      <c r="E20" s="1">
+        <v>184.83</v>
+      </c>
+      <c r="F20" s="1">
+        <v>1466327</v>
+      </c>
+      <c r="G20" s="1">
+        <f t="shared" si="4"/>
         <v>367500</v>
       </c>
-      <c r="D10" s="1">
-        <v>4.7190000000000003</v>
-      </c>
-      <c r="E10" s="1">
-        <v>114.85</v>
-      </c>
-      <c r="F10" s="1">
-        <f>2*C10-(A10+B10)</f>
-        <v>733775</v>
-      </c>
-      <c r="G10" s="1">
-        <f t="shared" si="1"/>
-        <v>1101275</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7">
-      <c r="A11" s="1">
-        <f t="shared" si="0"/>
-        <v>600</v>
-      </c>
-      <c r="B11" s="1">
-        <v>800</v>
-      </c>
-      <c r="C11" s="1">
-        <f>A11*B11</f>
-        <v>480000</v>
-      </c>
-      <c r="D11" s="1">
-        <v>6.141</v>
-      </c>
-      <c r="E11" s="1">
-        <v>166.4</v>
-      </c>
-      <c r="F11" s="1">
-        <f>2*C11-(A11+B11)</f>
-        <v>958600</v>
-      </c>
-      <c r="G11" s="1">
-        <f t="shared" si="1"/>
-        <v>1438600</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7">
-      <c r="A12" s="1">
-        <f t="shared" si="0"/>
-        <v>675</v>
-      </c>
-      <c r="B12" s="1">
-        <v>900</v>
-      </c>
-      <c r="C12" s="1">
-        <f>A12*B12</f>
-        <v>607500</v>
-      </c>
-      <c r="D12" s="1">
-        <v>7.532</v>
-      </c>
-      <c r="E12" s="1">
-        <v>206.1</v>
-      </c>
-      <c r="F12" s="1">
-        <f>2*C12-(A12+B12)</f>
-        <v>1213425</v>
-      </c>
-      <c r="G12" s="1">
-        <f t="shared" si="1"/>
-        <v>1820925</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7">
-      <c r="A13" s="1">
-        <f t="shared" si="0"/>
-        <v>750</v>
-      </c>
-      <c r="B13" s="1">
-        <v>1000</v>
-      </c>
-      <c r="C13" s="1">
-        <f>A13*B13</f>
-        <v>750000</v>
-      </c>
-      <c r="D13" s="1">
-        <v>11.484</v>
-      </c>
-      <c r="E13" s="1">
-        <v>242.55</v>
-      </c>
-      <c r="F13" s="1">
-        <f>2*C13-(A13+B13)</f>
-        <v>1498250</v>
-      </c>
-      <c r="G13" s="1">
-        <f t="shared" si="1"/>
-        <v>2248250</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7">
-      <c r="A14" s="1">
-        <f t="shared" si="0"/>
-        <v>825</v>
-      </c>
-      <c r="B14" s="1">
-        <v>1100</v>
-      </c>
-      <c r="C14" s="1">
-        <f>A14*B14</f>
-        <v>907500</v>
-      </c>
-      <c r="D14" s="1">
-        <v>13.452999999999999</v>
-      </c>
-      <c r="E14" s="1">
-        <v>313.92</v>
-      </c>
-      <c r="F14" s="1">
-        <f>2*C14-(A14+B14)</f>
-        <v>1813075</v>
-      </c>
-      <c r="G14" s="1">
-        <f t="shared" si="1"/>
-        <v>2720575</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7">
-      <c r="A15" s="1">
-        <f t="shared" si="0"/>
-        <v>900</v>
-      </c>
-      <c r="B15" s="1">
-        <v>1200</v>
-      </c>
-      <c r="C15" s="1">
-        <f>A15*B15</f>
-        <v>1080000</v>
-      </c>
-      <c r="D15" s="1">
-        <v>18.375</v>
-      </c>
-      <c r="E15" s="1">
-        <v>350.44</v>
-      </c>
-      <c r="F15" s="1">
-        <f>2*C15-(A15+B15)</f>
-        <v>2157900</v>
-      </c>
-      <c r="G15" s="1">
-        <f t="shared" si="1"/>
-        <v>3237900</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7">
-      <c r="A16" s="1">
-        <f t="shared" si="0"/>
-        <v>975</v>
-      </c>
-      <c r="B16" s="1">
-        <v>1300</v>
-      </c>
-      <c r="C16" s="1">
-        <f>A16*B16</f>
-        <v>1267500</v>
-      </c>
-      <c r="D16" s="1">
-        <v>20.327999999999999</v>
-      </c>
-      <c r="E16" s="1">
-        <v>425.84</v>
-      </c>
-      <c r="F16" s="1">
-        <f>2*C16-(A16+B16)</f>
-        <v>2532725</v>
-      </c>
-      <c r="G16" s="1">
-        <f t="shared" si="1"/>
-        <v>3800225</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7">
-      <c r="A17" s="1">
-        <f t="shared" si="0"/>
-        <v>1050</v>
-      </c>
-      <c r="B17" s="1">
-        <v>1400</v>
-      </c>
-      <c r="C17" s="1">
-        <f>A17*B17</f>
-        <v>1470000</v>
-      </c>
-      <c r="D17" s="1">
-        <v>22.859000000000002</v>
-      </c>
-      <c r="E17" s="1">
-        <v>489.75</v>
-      </c>
-      <c r="F17" s="1">
-        <f>2*C17-(A17+B17)</f>
-        <v>2937550</v>
-      </c>
-      <c r="G17" s="1">
-        <f t="shared" si="1"/>
-        <v>4407550</v>
+      <c r="H20" s="1">
+        <f t="shared" si="2"/>
+        <v>1833827</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B2:I2"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <drawing r:id="rId2"/>

</xml_diff>